<commit_message>
v26.2.1: Atualização de dados CSV (Faturamento e Contratos)
</commit_message>
<xml_diff>
--- a/Consolidado Faturamento.xlsx
+++ b/Consolidado Faturamento.xlsx
@@ -5,19 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marbrti.sharepoint.com/sites/financeirosite/Documentos Compartilhados/Gestão/Automações/DRE-V14-Contratos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicole\Mar Brasil\Financeiro - Documentos\Gestão\Automações\DRE-V14-Contratos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{7E040986-393F-4204-83B4-627E3E19C26C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6541419-03CB-4C3C-9218-E0330A564E7D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3D8480D-7662-47F0-974C-AD5BA64BE297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="615" xr2:uid="{34302E59-E231-43F7-8EB2-6BAE469C7CD7}"/>
+    <workbookView xWindow="360" yWindow="288" windowWidth="21600" windowHeight="11232" tabRatio="615" xr2:uid="{34302E59-E231-43F7-8EB2-6BAE469C7CD7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Matriz" sheetId="14" r:id="rId1"/>
+    <sheet name="Consolidado Faturamento" sheetId="14" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -209,7 +206,7 @@
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$-416]mmm\-yy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +231,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos"/>
       <family val="2"/>
     </font>
@@ -277,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -299,6 +303,9 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -564,48 +571,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Janeiro"/>
-      <sheetName val="Fevereiro"/>
-      <sheetName val="Março"/>
-      <sheetName val="Abril"/>
-      <sheetName val="Maio"/>
-      <sheetName val="Junho"/>
-      <sheetName val="Julho"/>
-      <sheetName val="Agosto"/>
-      <sheetName val="Setembro"/>
-      <sheetName val="Outubro"/>
-      <sheetName val="Novembro"/>
-      <sheetName val="Dezembro"/>
-      <sheetName val="Impostos"/>
-      <sheetName val="Inadimplência"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -947,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229272A8-34A2-4462-BE4D-F05BA25CDC34}">
   <dimension ref="A1:K219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="L172" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="H163" sqref="H163:J179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6629,17 +6594,14 @@
       <c r="G163" s="12">
         <v>45764</v>
       </c>
-      <c r="H163" s="13">
-        <f>[1]Impostos!E194</f>
-        <v>0</v>
-      </c>
-      <c r="I163" s="13">
-        <f t="shared" ref="I163:I179" si="0">H163-J163</f>
-        <v>0</v>
-      </c>
-      <c r="J163" s="13">
-        <f>[1]Impostos!L194</f>
-        <v>0</v>
+      <c r="H163" s="21">
+        <v>31583.33</v>
+      </c>
+      <c r="I163" s="21">
+        <v>26151.58894823194</v>
+      </c>
+      <c r="J163" s="21">
+        <v>5431.7410517680628</v>
       </c>
       <c r="K163" s="14" t="s">
         <v>10</v>
@@ -6667,17 +6629,14 @@
       <c r="G164" s="12">
         <v>45931</v>
       </c>
-      <c r="H164" s="13">
-        <f>[1]Impostos!E196</f>
-        <v>0</v>
-      </c>
-      <c r="I164" s="13">
-        <f>H164-J164</f>
-        <v>0</v>
-      </c>
-      <c r="J164" s="13">
-        <f>[1]Impostos!L196</f>
-        <v>0</v>
+      <c r="H164" s="21">
+        <v>6442.8</v>
+      </c>
+      <c r="I164" s="21">
+        <v>5875.9543047450898</v>
+      </c>
+      <c r="J164" s="21">
+        <v>566.84569525491042</v>
       </c>
       <c r="K164" s="14" t="s">
         <v>10</v>
@@ -6705,17 +6664,14 @@
       <c r="G165" s="12">
         <v>45757</v>
       </c>
-      <c r="H165" s="13">
-        <f>[1]Impostos!E190</f>
-        <v>0</v>
-      </c>
-      <c r="I165" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J165" s="13">
-        <f>[1]Impostos!L190</f>
-        <v>0</v>
+      <c r="H165" s="21">
+        <v>384217.38</v>
+      </c>
+      <c r="I165" s="21">
+        <v>318139.18888624571</v>
+      </c>
+      <c r="J165" s="21">
+        <v>66078.191113754292</v>
       </c>
       <c r="K165" s="14" t="s">
         <v>10</v>
@@ -6741,17 +6697,14 @@
       <c r="G166" s="12">
         <v>45742</v>
       </c>
-      <c r="H166" s="13">
-        <f>[1]Impostos!E193</f>
-        <v>0</v>
-      </c>
-      <c r="I166" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J166" s="13">
-        <f>[1]Impostos!L193</f>
-        <v>0</v>
+      <c r="H166" s="21">
+        <v>14441.02</v>
+      </c>
+      <c r="I166" s="21">
+        <v>12390.665710015201</v>
+      </c>
+      <c r="J166" s="21">
+        <v>2050.3542899847994</v>
       </c>
       <c r="K166" s="14" t="s">
         <v>10</v>
@@ -6777,15 +6730,13 @@
       <c r="G167" s="12">
         <v>45737</v>
       </c>
-      <c r="H167" s="13">
+      <c r="H167" s="21">
         <v>2280.11</v>
       </c>
-      <c r="I167" s="13">
-        <f t="shared" si="0"/>
+      <c r="I167" s="21">
         <v>1908.627266</v>
       </c>
-      <c r="J167" s="13">
-        <f>2853.17*0.1302</f>
+      <c r="J167" s="21">
         <v>371.48273400000005</v>
       </c>
       <c r="K167" s="14" t="s">
@@ -6812,15 +6763,13 @@
       <c r="G168" s="12">
         <v>45737</v>
       </c>
-      <c r="H168" s="13">
+      <c r="H168" s="21">
         <v>380</v>
       </c>
-      <c r="I168" s="13">
-        <f t="shared" si="0"/>
+      <c r="I168" s="21">
         <v>318.08621099999999</v>
       </c>
-      <c r="J168" s="13">
-        <f>2853.17*0.0217</f>
+      <c r="J168" s="21">
         <v>61.913789000000001</v>
       </c>
       <c r="K168" s="14" t="s">
@@ -6847,15 +6796,13 @@
       <c r="G169" s="12">
         <v>45737</v>
       </c>
-      <c r="H169" s="13">
+      <c r="H169" s="21">
         <v>830</v>
       </c>
-      <c r="I169" s="13">
-        <f t="shared" si="0"/>
+      <c r="I169" s="21">
         <v>694.75974199999996</v>
       </c>
-      <c r="J169" s="13">
-        <f>2853.17*0.0474</f>
+      <c r="J169" s="21">
         <v>135.24025799999998</v>
       </c>
       <c r="K169" s="14" t="s">
@@ -6882,15 +6829,13 @@
       <c r="G170" s="12">
         <v>45737</v>
       </c>
-      <c r="H170" s="13">
+      <c r="H170" s="21">
         <v>4108.59</v>
       </c>
-      <c r="I170" s="13">
-        <f t="shared" si="0"/>
+      <c r="I170" s="21">
         <v>3439.2363180000002</v>
       </c>
-      <c r="J170" s="13">
-        <f>2853.17*0.2346</f>
+      <c r="J170" s="21">
         <v>669.35368200000005</v>
       </c>
       <c r="K170" s="14" t="s">
@@ -6917,15 +6862,13 @@
       <c r="G171" s="12">
         <v>45737</v>
       </c>
-      <c r="H171" s="13">
+      <c r="H171" s="21">
         <v>6914</v>
       </c>
-      <c r="I171" s="13">
-        <f t="shared" si="0"/>
+      <c r="I171" s="21">
         <v>5787.2831669999996</v>
       </c>
-      <c r="J171" s="13">
-        <f>2853.17*0.3949</f>
+      <c r="J171" s="21">
         <v>1126.716833</v>
       </c>
       <c r="K171" s="14" t="s">
@@ -6952,15 +6895,13 @@
       <c r="G172" s="12">
         <v>45737</v>
       </c>
-      <c r="H172" s="13">
+      <c r="H172" s="21">
         <v>2996.94</v>
       </c>
-      <c r="I172" s="13">
-        <f t="shared" si="0"/>
+      <c r="I172" s="21">
         <v>2507.3360280000002</v>
       </c>
-      <c r="J172" s="13">
-        <f>2853.17*0.1716</f>
+      <c r="J172" s="21">
         <v>489.603972</v>
       </c>
       <c r="K172" s="14" t="s">
@@ -6987,17 +6928,14 @@
       <c r="G173" s="12">
         <v>45726</v>
       </c>
-      <c r="H173" s="13">
-        <f>[1]Impostos!E188</f>
-        <v>0</v>
-      </c>
-      <c r="I173" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J173" s="13">
-        <f>[1]Impostos!L188</f>
-        <v>0</v>
+      <c r="H173" s="21">
+        <v>800</v>
+      </c>
+      <c r="I173" s="21">
+        <v>686.41498786181035</v>
+      </c>
+      <c r="J173" s="21">
+        <v>113.58501213818965</v>
       </c>
       <c r="K173" s="14" t="s">
         <v>10</v>
@@ -7025,17 +6963,14 @@
       <c r="G174" s="12">
         <v>45707</v>
       </c>
-      <c r="H174" s="13">
-        <f>[1]Impostos!E192</f>
-        <v>0</v>
-      </c>
-      <c r="I174" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J174" s="13">
-        <f>[1]Impostos!L192</f>
-        <v>0</v>
+      <c r="H174" s="21">
+        <v>90410.05</v>
+      </c>
+      <c r="I174" s="21">
+        <v>77573.51671666959</v>
+      </c>
+      <c r="J174" s="21">
+        <v>12836.533283330416</v>
       </c>
       <c r="K174" s="14" t="s">
         <v>10</v>
@@ -7063,17 +6998,14 @@
       <c r="G175" s="12">
         <v>45625</v>
       </c>
-      <c r="H175" s="13">
-        <f>[1]Impostos!E191</f>
-        <v>0</v>
-      </c>
-      <c r="I175" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J175" s="13">
-        <f>[1]Impostos!L191</f>
-        <v>0</v>
+      <c r="H175" s="21">
+        <v>25651.74</v>
+      </c>
+      <c r="I175" s="21">
+        <v>22009.673500917896</v>
+      </c>
+      <c r="J175" s="21">
+        <v>3642.0664990821065</v>
       </c>
       <c r="K175" s="14" t="s">
         <v>10</v>
@@ -7099,15 +7031,13 @@
       <c r="G176" s="4">
         <v>45747</v>
       </c>
-      <c r="H176" s="5">
+      <c r="H176" s="22">
         <v>21402.22</v>
       </c>
-      <c r="I176" s="5">
-        <f t="shared" si="0"/>
+      <c r="I176" s="22">
         <v>19957.790316000002</v>
       </c>
-      <c r="J176" s="5">
-        <f>2909.81*0.4964</f>
+      <c r="J176" s="22">
         <v>1444.429684</v>
       </c>
       <c r="K176" s="6" t="s">
@@ -7134,15 +7064,13 @@
       <c r="G177" s="4">
         <v>45825</v>
       </c>
-      <c r="H177" s="5">
+      <c r="H177" s="22">
         <v>7184.3</v>
       </c>
-      <c r="I177" s="5">
-        <f t="shared" si="0"/>
+      <c r="I177" s="22">
         <v>6699.2346729999999</v>
       </c>
-      <c r="J177" s="5">
-        <f>2909.81*0.1667</f>
+      <c r="J177" s="22">
         <v>485.06532699999997</v>
       </c>
       <c r="K177" s="6" t="s">
@@ -7169,15 +7097,13 @@
       <c r="G178" s="4">
         <v>45734</v>
       </c>
-      <c r="H178" s="5">
+      <c r="H178" s="22">
         <v>14531.48</v>
       </c>
-      <c r="I178" s="5">
-        <f t="shared" si="0"/>
+      <c r="I178" s="22">
         <v>13550.874029999999</v>
       </c>
-      <c r="J178" s="5">
-        <f>2909.81*0.337</f>
+      <c r="J178" s="22">
         <v>980.60597000000007</v>
       </c>
       <c r="K178" s="6" t="s">
@@ -7206,14 +7132,13 @@
       <c r="G179" s="8">
         <v>45734</v>
       </c>
-      <c r="H179" s="9">
+      <c r="H179" s="23">
         <v>972.01</v>
       </c>
-      <c r="I179" s="9">
-        <f t="shared" si="0"/>
+      <c r="I179" s="23">
         <v>899.82999999999993</v>
       </c>
-      <c r="J179" s="9">
+      <c r="J179" s="23">
         <v>72.180000000000007</v>
       </c>
       <c r="K179" s="7" t="s">
@@ -8591,6 +8516,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b8ec653c-db26-4c1a-b2d8-4fc87e95ce94" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c34becbf-ca68-4256-8aed-b392b0a2c6fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DB710B410562E7408FD56977B2428FD4" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="7f3b8e69fc43edacbf3460c765d836bd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c34becbf-ca68-4256-8aed-b392b0a2c6fb" xmlns:ns3="b8ec653c-db26-4c1a-b2d8-4fc87e95ce94" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01daf5f34cc6c9db21582b6e7d6f6b2f" ns2:_="" ns3:_="">
     <xsd:import namespace="c34becbf-ca68-4256-8aed-b392b0a2c6fb"/>
@@ -8797,27 +8742,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b8ec653c-db26-4c1a-b2d8-4fc87e95ce94" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c34becbf-ca68-4256-8aed-b392b0a2c6fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3788B48-995E-4AB3-B316-5D60809EDD54}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EF121F4-8882-473B-91AF-F48CEAAD652A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b8ec653c-db26-4c1a-b2d8-4fc87e95ce94"/>
+    <ds:schemaRef ds:uri="c34becbf-ca68-4256-8aed-b392b0a2c6fb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0462A70-4274-4D6D-B24D-623BC7319EF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8834,23 +8778,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EF121F4-8882-473B-91AF-F48CEAAD652A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b8ec653c-db26-4c1a-b2d8-4fc87e95ce94"/>
-    <ds:schemaRef ds:uri="c34becbf-ca68-4256-8aed-b392b0a2c6fb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3788B48-995E-4AB3-B316-5D60809EDD54}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>